<commit_message>
FINALLY THE DATA ASSIM IS WORKING YAYYY!!!! WELL CHUFFED INNIT
</commit_message>
<xml_diff>
--- a/observeddata/Ebola_Death_Data_4zones.xlsx
+++ b/observeddata/Ebola_Death_Data_4zones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashok\Desktop\spatialEpisim2022\spatialEpisim\observeddata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhit957\Desktop\spatialEpisim\observeddata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC69C15-D4E8-41DC-9D98-9E88978866A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD29CA1-0E22-4834-982B-1E9379C87480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Death" sheetId="2" r:id="rId1"/>
@@ -479,20 +479,20 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -520,19 +520,19 @@
         <v>43682</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -592,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -692,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -732,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -812,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -832,7 +832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -952,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>

</xml_diff>